<commit_message>
Editing README, adding icon
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,64 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb3ri\Downloads\Tkinter\devlop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb3ri\Downloads\Tkinter\develop\Simple-Inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9364CE16-62D4-4F8D-AE7A-9B43588C324C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1A8B23-81BC-4611-8955-35FAEB20F3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
-  <si>
-    <t xml:space="preserve">First </t>
-  </si>
-  <si>
-    <t>Middle</t>
-  </si>
-  <si>
-    <t>Last</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Extra</t>
+    <t>CAS</t>
+  </si>
+  <si>
+    <t>108-24-7</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Acetic Acid</t>
+  </si>
+  <si>
+    <t>Hexane</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,10 +84,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -81,14 +122,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -111,44 +158,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -175,15 +222,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -210,7 +256,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -222,172 +267,199 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -398,10 +470,13 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -409,13 +484,13 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>4</v>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -426,8 +501,12 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>